<commit_message>
Recorded remainder of tests
</commit_message>
<xml_diff>
--- a/tests/Results.xlsx
+++ b/tests/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>LUT</t>
   </si>
@@ -78,14 +78,55 @@
   </si>
   <si>
     <t>Performance-Optimized, barrel shifter, integer multiplier (DSP Slice), divider, and branch target cache (5 Stage Pipeline)</t>
+  </si>
+  <si>
+    <t>Frequency-Optimized, otherwise matching implementation #1</t>
+  </si>
+  <si>
+    <t>Maximum Frequency - No cache, 5 stage pipeline, no mulplier/divider/caches. Intended to reach the maximum frequency</t>
+  </si>
+  <si>
+    <t>Minimum Area, no multiplier, divider, or branch predictor (3 Stage pipeline)</t>
+  </si>
+  <si>
+    <t>Maximum Frequency, otherwise matching implementation #1</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>** Dynamic power does not include power from PLL, which makes up ~101mW</t>
+  </si>
+  <si>
+    <t>Frequency-Optimized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum Performance - No i/d cache, 5 stage pipeline, multiper + branch cache </t>
+  </si>
+  <si>
+    <t>Area Optimized, includes mulitplier and barrel shifter (3 Stage pipeline)</t>
+  </si>
+  <si>
+    <t>2nd tests</t>
+  </si>
+  <si>
+    <t>pt2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -113,8 +154,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,132 +487,413 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>1590</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>1359</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>0</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>75</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>25</v>
       </c>
-      <c r="H4">
+      <c r="G4" s="1">
+        <v>100</v>
+      </c>
+      <c r="H4" s="1">
         <v>0.55800000000000005</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1">
         <v>0.70599999999999996</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="1">
+        <f>H4+I4</f>
         <v>1.264</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>2316</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>2071</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>3</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>75</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>43</v>
       </c>
-      <c r="H5">
+      <c r="G5" s="1">
+        <v>100</v>
+      </c>
+      <c r="H5" s="1">
         <v>0.52500000000000002</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="1">
         <v>0.66300000000000003</v>
       </c>
-      <c r="J5">
-        <f>H5+I5</f>
+      <c r="J5" s="1">
+        <f t="shared" ref="J5:J13" si="0">H5+I5</f>
         <v>1.1880000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
+      <c r="B6" s="1">
+        <v>2365</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2420</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>75</v>
+      </c>
+      <c r="F6" s="1">
+        <v>21</v>
+      </c>
+      <c r="G6" s="1">
+        <v>100</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1.22</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1.296</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="0"/>
+        <v>2.516</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1530</v>
+      </c>
+      <c r="C9">
+        <v>1359</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>75</v>
+      </c>
+      <c r="F9">
+        <v>49</v>
+      </c>
+      <c r="G9">
+        <v>125</v>
+      </c>
+      <c r="H9">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="I9">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>1.0109999999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>3166</v>
+      </c>
+      <c r="C10">
+        <v>3222</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>75</v>
+      </c>
+      <c r="F10">
+        <v>57</v>
+      </c>
+      <c r="G10">
+        <v>125</v>
+      </c>
+      <c r="H10">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="I10">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>1.4870000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>2316</v>
+      </c>
+      <c r="C11">
+        <v>2071</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>75</v>
+      </c>
+      <c r="F11">
+        <v>43</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="I11">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ref="J11" si="1">H11+I11</f>
+        <v>1.1880000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>1881</v>
+      </c>
+      <c r="C12">
+        <v>1717</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>75</v>
+      </c>
+      <c r="F12">
+        <v>69</v>
+      </c>
+      <c r="G12">
+        <v>125</v>
+      </c>
+      <c r="H12">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="I12">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>1.095</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>1739</v>
+      </c>
+      <c r="C13">
+        <v>1510</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>75</v>
+      </c>
+      <c r="F13">
+        <v>68</v>
+      </c>
+      <c r="G13">
+        <v>125</v>
+      </c>
+      <c r="H13">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="I13">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>1.0069999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C22" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
         <v>2</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C23" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19">
+      <c r="C24" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="C25" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34">
         <v>1</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C34" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35">
         <v>2</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C35" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated power results and documentation
</commit_message>
<xml_diff>
--- a/tests/Results.xlsx
+++ b/tests/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
   <si>
     <t>All tests performed on  Xilinx 7s50csga324 device</t>
   </si>
@@ -191,16 +191,16 @@
     <t>PPW Real Delta Power</t>
   </si>
   <si>
-    <t>Board &amp; System</t>
+    <t>Measured Power</t>
   </si>
   <si>
-    <t>Static &amp; Dynamic</t>
+    <t>Board &amp; System Power</t>
   </si>
   <si>
-    <t>Vivado Estimated</t>
+    <t>Vivado Estimated Power</t>
   </si>
   <si>
-    <t>Measured Static + Dynamic</t>
+    <t>Device Power</t>
   </si>
 </sst>
 </file>
@@ -600,11 +600,265 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="345940280"/>
-        <c:axId val="345941064"/>
+        <c:axId val="182014176"/>
+        <c:axId val="348116168"/>
       </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.1282051282051294E-2"/>
+                  <c:y val="-3.2407407407407406E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.7315233785822019E-2"/>
+                  <c:y val="-3.2407407407407406E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.636500754147813E-2"/>
+                  <c:y val="-3.2407407407407406E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.6365007541478241E-2"/>
+                  <c:y val="-3.2407407407407447E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.1282051282051391E-2"/>
+                  <c:y val="-3.2407407407407406E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.731523378582213E-2"/>
+                  <c:y val="-3.2407407407407406E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$O$4:$T$4</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3 Stage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 Stage w/ Multiplier &amp; Divider</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5 Stage</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5 Stage w/ Multiplier</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5 Stage w/ Multiplier and Divider</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5 Stage w/ Multiplier &amp; Divider &amp; BTB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$7:$T$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>12.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1749999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.298</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.193999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.84</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.444</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="182014176"/>
+        <c:axId val="348116168"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="345940280"/>
+        <c:axId val="182014176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,7 +883,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345941064"/>
+        <c:crossAx val="348116168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -637,7 +891,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="345941064"/>
+        <c:axId val="348116168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -676,7 +930,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345940280"/>
+        <c:crossAx val="182014176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -688,6 +942,10 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
@@ -1012,11 +1270,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="345936360"/>
-        <c:axId val="345941456"/>
+        <c:axId val="348118520"/>
+        <c:axId val="348113816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="345936360"/>
+        <c:axId val="348118520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1041,7 +1299,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345941456"/>
+        <c:crossAx val="348113816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1049,7 +1307,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="345941456"/>
+        <c:axId val="348113816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,7 +1346,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345936360"/>
+        <c:crossAx val="348118520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1546,11 +1804,265 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="345937536"/>
-        <c:axId val="345941848"/>
+        <c:axId val="348118128"/>
+        <c:axId val="348118912"/>
       </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5146726862302484E-2"/>
+                  <c:y val="-3.2407407407407447E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5146726862302484E-2"/>
+                  <c:y val="-3.7037037037037035E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5146726862302484E-2"/>
+                  <c:y val="-3.2407407407407406E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5146726862302596E-2"/>
+                  <c:y val="-3.2407407407407406E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.8156508653122758E-2"/>
+                  <c:y val="-3.2407407407407447E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.8156508653122758E-2"/>
+                  <c:y val="-3.7037037037037035E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$O$16:$T$16</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3 Stage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 Stage w/ Multiplier &amp; Divider</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5 Stage</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5 Stage w/ Multiplier</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5 Stage w/ Multiplier and Divider</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5 Stage w/ Multiplier &amp; Divider &amp; BTB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$20:$T$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>235</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="348118128"/>
+        <c:axId val="348118912"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="345937536"/>
+        <c:axId val="348118128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1575,7 +2087,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345941848"/>
+        <c:crossAx val="348118912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1583,7 +2095,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="345941848"/>
+        <c:axId val="348118912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1622,7 +2134,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345937536"/>
+        <c:crossAx val="348118128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1634,6 +2146,10 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
@@ -1958,11 +2474,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="345937928"/>
-        <c:axId val="345943024"/>
+        <c:axId val="348116560"/>
+        <c:axId val="348119304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="345937928"/>
+        <c:axId val="348116560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1987,7 +2503,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345943024"/>
+        <c:crossAx val="348119304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1995,7 +2511,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="345943024"/>
+        <c:axId val="348119304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2034,7 +2550,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345937928"/>
+        <c:crossAx val="348116560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2249,11 +2765,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="345942632"/>
-        <c:axId val="345939104"/>
+        <c:axId val="348117344"/>
+        <c:axId val="348114208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="345942632"/>
+        <c:axId val="348117344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2278,7 +2794,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345939104"/>
+        <c:crossAx val="348114208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2286,7 +2802,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="345939104"/>
+        <c:axId val="348114208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2325,7 +2841,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345942632"/>
+        <c:crossAx val="348117344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2399,7 +2915,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Vivado Estimated</c:v>
+                  <c:v>Vivado Estimated Power</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2520,11 +3036,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="346554384"/>
-        <c:axId val="346551248"/>
+        <c:axId val="348113424"/>
+        <c:axId val="348114992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="346554384"/>
+        <c:axId val="348113424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2549,7 +3065,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346551248"/>
+        <c:crossAx val="348114992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2557,7 +3073,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="346551248"/>
+        <c:axId val="348114992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2596,7 +3112,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346554384"/>
+        <c:crossAx val="348113424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2677,7 +3193,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Board &amp; System</c:v>
+                  <c:v>Board &amp; System Power</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2798,7 +3314,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Static &amp; Dynamic</c:v>
+                  <c:v>Device Power</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2920,11 +3436,265 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="473041296"/>
-        <c:axId val="473040120"/>
+        <c:axId val="348115776"/>
+        <c:axId val="348112640"/>
       </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.8156508653122647E-2"/>
+                  <c:y val="-3.2407407407407447E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5146726862302484E-2"/>
+                  <c:y val="-3.2407407407407406E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5146726862302484E-2"/>
+                  <c:y val="-3.2407407407407406E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5146726862302596E-2"/>
+                  <c:y val="-3.2407407407407406E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5146726862302596E-2"/>
+                  <c:y val="-3.2407407407407406E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5146726862302373E-2"/>
+                  <c:y val="-3.7037037037037077E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$O$30:$T$30</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3 Stage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 Stage w/ Multiplier &amp; Divider</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5 Stage</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5 Stage w/ Multiplier</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5 Stage w/ Multiplier and Divider</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5 Stage w/ Multiplier &amp; Divider &amp; BTB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$33:$T$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>925</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>928</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>937</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>933</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>753</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="348115776"/>
+        <c:axId val="348112640"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="473041296"/>
+        <c:axId val="348115776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2949,7 +3719,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="473040120"/>
+        <c:crossAx val="348112640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2957,7 +3727,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="473040120"/>
+        <c:axId val="348112640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2996,7 +3766,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="473041296"/>
+        <c:crossAx val="348115776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3008,6 +3778,10 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
@@ -3102,7 +3876,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Vivado Estimated</c:v>
+                  <c:v>Vivado Estimated Power</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3225,7 +3999,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Measured Static + Dynamic</c:v>
+                  <c:v>Measured Power</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3306,22 +4080,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>27.87</c:v>
+                  <c:v>14.31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>220.35</c:v>
+                  <c:v>109.79</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.43</c:v>
+                  <c:v>13.77</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.11</c:v>
+                  <c:v>17.52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>127.59</c:v>
+                  <c:v>63.57</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>208.69</c:v>
+                  <c:v>103.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3347,11 +4121,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="473046000"/>
-        <c:axId val="473039728"/>
+        <c:axId val="348882400"/>
+        <c:axId val="348883184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="473046000"/>
+        <c:axId val="348882400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3376,7 +4150,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="473039728"/>
+        <c:crossAx val="348883184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3384,7 +4158,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="473039728"/>
+        <c:axId val="348883184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3423,7 +4197,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="473046000"/>
+        <c:crossAx val="348882400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3944,8 +4718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P94" sqref="P94"/>
+    <sheetView tabSelected="1" topLeftCell="G22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4883,7 +5657,7 @@
         <v>44</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="O31">
         <v>570</v>
@@ -4906,7 +5680,7 @@
     </row>
     <row r="32" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N32" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="O32">
         <v>355</v>
@@ -4930,6 +5704,33 @@
     <row r="33" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>45</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O33">
+        <f>O31+O32</f>
+        <v>925</v>
+      </c>
+      <c r="P33">
+        <f t="shared" ref="P33:T33" si="3">P31+P32</f>
+        <v>758</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="3"/>
+        <v>928</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="3"/>
+        <v>937</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="3"/>
+        <v>933</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="3"/>
+        <v>753</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5031,57 +5832,57 @@
         <v>57</v>
       </c>
       <c r="O44">
-        <f>ROUND((2^16/O7)/O20,2)</f>
+        <f t="shared" ref="O44:T44" si="4">ROUND((2^16/O7)/O20,2)</f>
         <v>22.58</v>
       </c>
       <c r="P44">
-        <f>ROUND((2^16/P7)/P20,2)</f>
+        <f t="shared" si="4"/>
         <v>90.93</v>
       </c>
       <c r="Q44">
-        <f>ROUND((2^16/Q7)/Q20,2)</f>
+        <f t="shared" si="4"/>
         <v>18.670000000000002</v>
       </c>
       <c r="R44">
-        <f>ROUND((2^16/R7)/R20,2)</f>
+        <f t="shared" si="4"/>
         <v>24.35</v>
       </c>
       <c r="S44">
-        <f>ROUND((2^16/S7)/S20,2)</f>
+        <f t="shared" si="4"/>
         <v>91.21</v>
       </c>
       <c r="T44">
-        <f>ROUND((2^16/T7)/T20,2)</f>
+        <f t="shared" si="4"/>
         <v>80.97</v>
       </c>
     </row>
     <row r="45" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N45" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="O45">
-        <f>ROUND((2^16/O32)/O6,2)</f>
-        <v>27.87</v>
+        <f>ROUND((2^16/O7)/O32,2)</f>
+        <v>14.31</v>
       </c>
       <c r="P45">
-        <f>ROUND((2^16/P32)/P6,2)</f>
-        <v>220.35</v>
+        <f>ROUND((2^16/P7)/P32,2)</f>
+        <v>109.79</v>
       </c>
       <c r="Q45">
-        <f>ROUND((2^16/Q32)/Q6,2)</f>
-        <v>28.43</v>
+        <f t="shared" ref="Q45:T45" si="5">ROUND((2^16/Q7)/Q32,2)</f>
+        <v>13.77</v>
       </c>
       <c r="R45">
-        <f>ROUND((2^16/R32)/R6,2)</f>
-        <v>34.11</v>
+        <f t="shared" si="5"/>
+        <v>17.52</v>
       </c>
       <c r="S45">
-        <f>ROUND((2^16/S32)/S6,2)</f>
-        <v>127.59</v>
+        <f t="shared" si="5"/>
+        <v>63.57</v>
       </c>
       <c r="T45">
-        <f>ROUND((2^16/T32)/T6,2)</f>
-        <v>208.69</v>
+        <f t="shared" si="5"/>
+        <v>103.98</v>
       </c>
     </row>
     <row r="46" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated results with more accurate power estimations. Updated documentation
</commit_message>
<xml_diff>
--- a/tests/Results.xlsx
+++ b/tests/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="66">
   <si>
     <t>All tests performed on  Xilinx 7s50csga324 device</t>
   </si>
@@ -197,10 +197,31 @@
     <t>Board &amp; System Power</t>
   </si>
   <si>
-    <t>Vivado Estimated Power</t>
+    <t>Device Power</t>
   </si>
   <si>
-    <t>Device Power</t>
+    <t>Vivado Estimated</t>
+  </si>
+  <si>
+    <t>Measured</t>
+  </si>
+  <si>
+    <t>Estimated Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power </t>
+  </si>
+  <si>
+    <t>Junction Temp</t>
+  </si>
+  <si>
+    <t>15.1 C/W</t>
+  </si>
+  <si>
+    <t>Effective tresistance</t>
+  </si>
+  <si>
+    <t>New dynamic</t>
   </si>
 </sst>
 </file>
@@ -600,8 +621,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="182014176"/>
-        <c:axId val="348116168"/>
+        <c:axId val="1095984"/>
+        <c:axId val="337029280"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -784,7 +805,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -854,11 +874,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="182014176"/>
-        <c:axId val="348116168"/>
+        <c:axId val="1095984"/>
+        <c:axId val="337029280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="182014176"/>
+        <c:axId val="1095984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -883,7 +903,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348116168"/>
+        <c:crossAx val="337029280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -891,7 +911,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348116168"/>
+        <c:axId val="337029280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -930,7 +950,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="182014176"/>
+        <c:crossAx val="1095984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1270,11 +1290,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="348118520"/>
-        <c:axId val="348113816"/>
+        <c:axId val="337031632"/>
+        <c:axId val="337026144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="348118520"/>
+        <c:axId val="337031632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1299,7 +1319,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348113816"/>
+        <c:crossAx val="337026144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1307,7 +1327,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348113816"/>
+        <c:axId val="337026144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1346,7 +1366,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348118520"/>
+        <c:crossAx val="337031632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1416,7 +1436,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Vivado Estimated Power Utilization per Implementation (mW)</a:t>
+              <a:t>Vivado Estimated Power Utilization per Implementation (mW) (out of date)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1804,8 +1824,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="348118128"/>
-        <c:axId val="348118912"/>
+        <c:axId val="337027712"/>
+        <c:axId val="337029672"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1988,7 +2008,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -2058,11 +2077,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="348118128"/>
-        <c:axId val="348118912"/>
+        <c:axId val="337027712"/>
+        <c:axId val="337029672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="348118128"/>
+        <c:axId val="337027712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2087,7 +2106,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348118912"/>
+        <c:crossAx val="337029672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2095,7 +2114,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348118912"/>
+        <c:axId val="337029672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2134,7 +2153,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348118128"/>
+        <c:crossAx val="337027712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2474,11 +2493,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="348116560"/>
-        <c:axId val="348119304"/>
+        <c:axId val="337027320"/>
+        <c:axId val="337024576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="348116560"/>
+        <c:axId val="337027320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2503,7 +2522,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348119304"/>
+        <c:crossAx val="337024576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2511,7 +2530,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348119304"/>
+        <c:axId val="337024576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2550,7 +2569,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348116560"/>
+        <c:crossAx val="337027320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2765,11 +2784,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="348117344"/>
-        <c:axId val="348114208"/>
+        <c:axId val="337024968"/>
+        <c:axId val="337025752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="348117344"/>
+        <c:axId val="337024968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2794,7 +2813,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348114208"/>
+        <c:crossAx val="337025752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2802,7 +2821,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348114208"/>
+        <c:axId val="337025752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2841,7 +2860,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348117344"/>
+        <c:crossAx val="337024968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2869,277 +2888,6 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="1"/>
-  <c:style val="2"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr sz="1400" b="0" i="0">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Performance Per Watt (kB/s per W)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$N$44</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Vivado Estimated Power</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5B9BD5"/>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="1"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr sz="900" b="0" i="0">
-                    <a:solidFill>
-                      <a:srgbClr val="404040"/>
-                    </a:solidFill>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$O$43:$T$43</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3 Stage</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3 Stage w/ Multiplier &amp; Divider</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5 Stage</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5 Stage w/ Multiplier</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5 Stage w/ Multiplier and Divider</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5 Stage w/ Multiplier &amp; Divider &amp; BTB</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$O$44:$T$44</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>22.58</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>90.93</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18.670000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>24.35</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>91.21</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>80.97</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
-              <c14:invertSolidFillFmt>
-                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </c14:spPr>
-              </c14:invertSolidFillFmt>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="348113424"/>
-        <c:axId val="348114992"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="348113424"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr sz="900" b="0" i="0">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="348114992"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="348114992"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="47625">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr sz="900" b="0" i="0">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="348113424"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3436,8 +3184,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="348115776"/>
-        <c:axId val="348112640"/>
+        <c:axId val="337028104"/>
+        <c:axId val="337030456"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3620,7 +3368,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -3690,11 +3437,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="348115776"/>
-        <c:axId val="348112640"/>
+        <c:axId val="337028104"/>
+        <c:axId val="337030456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="348115776"/>
+        <c:axId val="337028104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3719,7 +3466,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348112640"/>
+        <c:crossAx val="337030456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3727,7 +3474,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348112640"/>
+        <c:axId val="337030456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3766,7 +3513,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348115776"/>
+        <c:crossAx val="337028104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3782,6 +3529,433 @@
         <c:idx val="2"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr sz="900">
+              <a:solidFill>
+                <a:srgbClr val="595959"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1400" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Performance</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Per Watt (kB/s per W)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vivado Estimated</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5B9BD5"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="1"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr sz="900" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="404040"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$O$43:$T$43</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3 Stage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 Stage w/ Multiplier &amp; Divider</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5 Stage</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5 Stage w/ Multiplier</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5 Stage w/ Multiplier and Divider</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5 Stage w/ Multiplier &amp; Divider &amp; BTB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$44:$T$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>19.39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>81.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67.72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Measured</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ED7D31"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="1"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr sz="900" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="404040"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$O$43:$T$43</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3 Stage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 Stage w/ Multiplier &amp; Divider</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5 Stage</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5 Stage w/ Multiplier</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5 Stage w/ Multiplier and Divider</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5 Stage w/ Multiplier &amp; Divider &amp; BTB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$45:$T$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>14.31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>109.79</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.77</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>63.57</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>103.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="337832664"/>
+        <c:axId val="337831880"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="337832664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="900" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="337831880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="337831880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="D9D9D9"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="900" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="337832664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
@@ -3846,12 +4020,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Performance</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Per Watt (kB/s per W)</a:t>
+              <a:t>Device Power Utilization (mW)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -3872,11 +4042,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$44</c:f>
+              <c:f>Sheet1!$N$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Vivado Estimated Power</c:v>
+                  <c:v>Measured Power</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3927,7 +4097,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$O$43:$T$43</c:f>
+              <c:f>Sheet1!$O$35:$T$35</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -3953,27 +4123,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$44:$T$44</c:f>
+              <c:f>Sheet1!$O$36:$T$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>22.58</c:v>
+                  <c:v>355</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90.93</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.670000000000002</c:v>
+                  <c:v>358</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.35</c:v>
+                  <c:v>367</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91.21</c:v>
+                  <c:v>363</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.97</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3995,11 +4165,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$45</c:f>
+              <c:f>Sheet1!$N$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Measured Power</c:v>
+                  <c:v>Estimated Power</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4049,7 +4219,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$O$43:$T$43</c:f>
+              <c:f>Sheet1!$O$35:$T$35</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -4075,27 +4245,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$45:$T$45</c:f>
+              <c:f>Sheet1!$O$37:$T$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>14.31</c:v>
+                  <c:v>262</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>109.79</c:v>
+                  <c:v>275</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.77</c:v>
+                  <c:v>280</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.52</c:v>
+                  <c:v>304</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>63.57</c:v>
+                  <c:v>284</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>103.98</c:v>
+                  <c:v>281</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4121,11 +4291,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="348882400"/>
-        <c:axId val="348883184"/>
+        <c:axId val="337833840"/>
+        <c:axId val="337838544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="348882400"/>
+        <c:axId val="337833840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4150,7 +4320,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348883184"/>
+        <c:crossAx val="337838544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4158,7 +4328,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348883184"/>
+        <c:axId val="337838544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4197,7 +4367,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348882400"/>
+        <c:crossAx val="337833840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4209,6 +4379,804 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr sz="900">
+              <a:solidFill>
+                <a:srgbClr val="595959"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1400" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Vivado Estimated Power Utilization per Implementation (mW)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$57</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Phase Locked Loop Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="5B9BD5"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="1"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr sz="900" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="404040"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$O$56:$T$56</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3 Stage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 Stage w/ Multiplier &amp; Divider</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5 Stage</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5 Stage w/ Multiplier</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5 Stage w/ Multiplier and Divider</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5 Stage w/ Multiplier &amp; Divider &amp; BTB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$57:$T$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>103</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$58</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Static Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ED7D31"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="1"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr sz="900" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="404040"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$O$56:$T$56</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3 Stage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 Stage w/ Multiplier &amp; Divider</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5 Stage</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5 Stage w/ Multiplier</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5 Stage w/ Multiplier and Divider</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5 Stage w/ Multiplier &amp; Divider &amp; BTB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$58:$T$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$59</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dynamic Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF9900"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="1"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr sz="900" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="434343"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$O$56:$T$56</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3 Stage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 Stage w/ Multiplier &amp; Divider</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5 Stage</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5 Stage w/ Multiplier</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5 Stage w/ Multiplier and Divider</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5 Stage w/ Multiplier &amp; Divider &amp; BTB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$59:$T$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="442885128"/>
+        <c:axId val="442879248"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$60</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5146726862302484E-2"/>
+                  <c:y val="-3.2407407407407447E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5146726862302484E-2"/>
+                  <c:y val="-3.7037037037037035E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5146726862302484E-2"/>
+                  <c:y val="-3.2407407407407406E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5146726862302596E-2"/>
+                  <c:y val="-3.2407407407407406E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.8156508653122758E-2"/>
+                  <c:y val="-3.2407407407407447E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.8156508653122758E-2"/>
+                  <c:y val="-3.7037037037037035E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$O$56:$T$56</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3 Stage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 Stage w/ Multiplier &amp; Divider</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5 Stage</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5 Stage w/ Multiplier</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5 Stage w/ Multiplier and Divider</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5 Stage w/ Multiplier &amp; Divider &amp; BTB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$60:$T$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>281</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="442885128"/>
+        <c:axId val="442879248"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="442885128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="900" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="442879248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="442879248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="D9D9D9"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="900" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="442885128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
@@ -4374,31 +5342,6 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="4229100" cy="2743200"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="246354416" name="Chart 6" title="Chart"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
       <xdr:colOff>324971</xdr:colOff>
       <xdr:row>97</xdr:row>
       <xdr:rowOff>156883</xdr:rowOff>
@@ -4417,7 +5360,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4444,7 +5387,61 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4229100" cy="2743200"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 4" title="Chart"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4219575" cy="2743200"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 3" title="Chart"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4718,8 +5715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView tabSelected="1" topLeftCell="L45" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T60" sqref="T60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5410,11 +6407,11 @@
         <v>35</v>
       </c>
       <c r="O20">
-        <f t="shared" ref="O20:T20" si="2">O17+O18+O19</f>
+        <f>O17+O18+O19</f>
         <v>225</v>
       </c>
       <c r="P20">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="P20:T20" si="2">P17+P18+P19</f>
         <v>227</v>
       </c>
       <c r="Q20">
@@ -5680,7 +6677,7 @@
     </row>
     <row r="32" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N32" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O32">
         <v>355</v>
@@ -5747,6 +6744,24 @@
       </c>
       <c r="B35" t="s">
         <v>48</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5761,6 +6776,27 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
+      <c r="N36" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="O36">
+        <v>355</v>
+      </c>
+      <c r="P36">
+        <v>188</v>
+      </c>
+      <c r="Q36">
+        <v>358</v>
+      </c>
+      <c r="R36">
+        <v>367</v>
+      </c>
+      <c r="S36">
+        <v>363</v>
+      </c>
+      <c r="T36">
+        <v>183</v>
+      </c>
     </row>
     <row r="37" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
@@ -5774,6 +6810,33 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
+      <c r="N37" t="s">
+        <v>60</v>
+      </c>
+      <c r="O37">
+        <f>O60</f>
+        <v>262</v>
+      </c>
+      <c r="P37">
+        <f t="shared" ref="P37:T37" si="4">P60</f>
+        <v>275</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="4"/>
+        <v>280</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="4"/>
+        <v>304</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="4"/>
+        <v>284</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="4"/>
+        <v>281</v>
+      </c>
     </row>
     <row r="38" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5829,36 +6892,36 @@
     </row>
     <row r="44" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N44" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O44">
-        <f t="shared" ref="O44:T44" si="4">ROUND((2^16/O7)/O20,2)</f>
-        <v>22.58</v>
+        <f>ROUND((2^16/O7)/O60,2)</f>
+        <v>19.39</v>
       </c>
       <c r="P44">
-        <f t="shared" si="4"/>
-        <v>90.93</v>
+        <f t="shared" ref="P44:T44" si="5">ROUND((2^16/P7)/P60,2)</f>
+        <v>75.06</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="4"/>
-        <v>18.670000000000002</v>
+        <f t="shared" si="5"/>
+        <v>17.600000000000001</v>
       </c>
       <c r="R44">
-        <f t="shared" si="4"/>
-        <v>24.35</v>
+        <f t="shared" si="5"/>
+        <v>21.15</v>
       </c>
       <c r="S44">
-        <f t="shared" si="4"/>
-        <v>91.21</v>
+        <f t="shared" si="5"/>
+        <v>81.25</v>
       </c>
       <c r="T44">
-        <f t="shared" si="4"/>
-        <v>80.97</v>
+        <f t="shared" si="5"/>
+        <v>67.72</v>
       </c>
     </row>
     <row r="45" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N45" s="7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="O45">
         <f>ROUND((2^16/O7)/O32,2)</f>
@@ -5869,57 +6932,195 @@
         <v>109.79</v>
       </c>
       <c r="Q45">
-        <f t="shared" ref="Q45:T45" si="5">ROUND((2^16/Q7)/Q32,2)</f>
+        <f t="shared" ref="Q45:T45" si="6">ROUND((2^16/Q7)/Q32,2)</f>
         <v>13.77</v>
       </c>
       <c r="R45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>17.52</v>
       </c>
       <c r="S45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>63.57</v>
       </c>
       <c r="T45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>103.98</v>
       </c>
     </row>
     <row r="46" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="14:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="14:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="14:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="14:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="14:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="14:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="14:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="14:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T56" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="14:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N57" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O57" s="1">
+        <v>101</v>
+      </c>
+      <c r="P57" s="1">
+        <v>104</v>
+      </c>
+      <c r="Q57" s="1">
+        <v>101</v>
+      </c>
+      <c r="R57" s="1">
+        <v>101</v>
+      </c>
+      <c r="S57" s="1">
+        <v>101</v>
+      </c>
+      <c r="T57" s="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="14:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N58" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O58">
+        <v>96</v>
+      </c>
+      <c r="P58">
+        <v>96</v>
+      </c>
+      <c r="Q58">
+        <v>96</v>
+      </c>
+      <c r="R58">
+        <v>96</v>
+      </c>
+      <c r="S58">
+        <v>96</v>
+      </c>
+      <c r="T58">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="59" spans="14:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N59" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O59">
+        <v>65</v>
+      </c>
+      <c r="P59">
+        <v>75</v>
+      </c>
+      <c r="Q59">
+        <v>83</v>
+      </c>
+      <c r="R59">
+        <v>107</v>
+      </c>
+      <c r="S59">
+        <v>87</v>
+      </c>
+      <c r="T59">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="14:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N60" t="s">
+        <v>35</v>
+      </c>
+      <c r="O60">
+        <f>O57+O58+O59</f>
+        <v>262</v>
+      </c>
+      <c r="P60">
+        <f t="shared" ref="P60:T60" si="7">P57+P58+P59</f>
+        <v>275</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="7"/>
+        <v>280</v>
+      </c>
+      <c r="R60">
+        <f t="shared" si="7"/>
+        <v>304</v>
+      </c>
+      <c r="S60">
+        <f t="shared" si="7"/>
+        <v>284</v>
+      </c>
+      <c r="T60">
+        <f t="shared" si="7"/>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="61" spans="14:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="14:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N62" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q62">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="14:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="14:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="15:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="15:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="15:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O67" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" spans="15:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O68" t="s">
+        <v>62</v>
+      </c>
+      <c r="P68">
+        <v>50.3</v>
+      </c>
+    </row>
+    <row r="69" spans="15:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O69" t="s">
+        <v>64</v>
+      </c>
+      <c r="P69" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="70" spans="15:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="15:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="15:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="15:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="15:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="15:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="15:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="15:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="15:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="15:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="15:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>